<commit_message>
Added server role to background info
</commit_message>
<xml_diff>
--- a/servicelists/Service List.xlsx
+++ b/servicelists/Service List.xlsx
@@ -268,9 +268,6 @@
     <t>Any</t>
   </si>
   <si>
-    <t>Pub</t>
-  </si>
-  <si>
     <t>Cisco SIP Proxy</t>
   </si>
   <si>
@@ -347,6 +344,9 @@
   </si>
   <si>
     <t>Cisco RCC Device Selection Service</t>
+  </si>
+  <si>
+    <t>Publisher</t>
   </si>
 </sst>
 </file>
@@ -702,7 +702,7 @@
   <dimension ref="A1:G132"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F74" sqref="F74"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,7 +760,7 @@
         <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="D3" t="s">
         <v>34</v>
@@ -1015,7 +1015,7 @@
         <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="D18" t="s">
         <v>34</v>
@@ -1032,7 +1032,7 @@
         <v>33</v>
       </c>
       <c r="C19" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="D19" t="s">
         <v>34</v>
@@ -1100,7 +1100,7 @@
         <v>33</v>
       </c>
       <c r="C23" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="D23" t="s">
         <v>34</v>
@@ -1117,7 +1117,7 @@
         <v>33</v>
       </c>
       <c r="C24" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="D24" t="s">
         <v>34</v>
@@ -1855,7 +1855,7 @@
         <v>13</v>
       </c>
       <c r="B75" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C75" t="s">
         <v>83</v>
@@ -1872,7 +1872,7 @@
         <v>15</v>
       </c>
       <c r="B76" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C76" t="s">
         <v>83</v>
@@ -1889,7 +1889,7 @@
         <v>17</v>
       </c>
       <c r="B77" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C77" t="s">
         <v>83</v>
@@ -1903,10 +1903,10 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B78" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C78" t="s">
         <v>83</v>
@@ -1920,10 +1920,10 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B79" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C79" t="s">
         <v>83</v>
@@ -1937,10 +1937,10 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B80" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C80" t="s">
         <v>83</v>
@@ -1954,10 +1954,10 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B81" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C81" t="s">
         <v>83</v>
@@ -1971,10 +1971,10 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B82" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C82" t="s">
         <v>83</v>
@@ -1988,10 +1988,10 @@
     </row>
     <row r="83" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B83" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C83" t="s">
         <v>83</v>
@@ -2005,10 +2005,10 @@
     </row>
     <row r="84" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B84" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C84" t="s">
         <v>83</v>
@@ -2022,10 +2022,10 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B85" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C85" t="s">
         <v>83</v>
@@ -2039,10 +2039,10 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B86" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C86" t="s">
         <v>83</v>
@@ -2056,10 +2056,10 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B87" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C87" t="s">
         <v>83</v>
@@ -2076,7 +2076,7 @@
         <v>29</v>
       </c>
       <c r="B88" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C88" t="s">
         <v>83</v>
@@ -2090,7 +2090,7 @@
         <v>35</v>
       </c>
       <c r="B89" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C89" t="s">
         <v>83</v>
@@ -2104,7 +2104,7 @@
         <v>36</v>
       </c>
       <c r="B90" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C90" t="s">
         <v>83</v>
@@ -2118,7 +2118,7 @@
         <v>37</v>
       </c>
       <c r="B91" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C91" t="s">
         <v>83</v>
@@ -2132,7 +2132,7 @@
         <v>38</v>
       </c>
       <c r="B92" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C92" t="s">
         <v>83</v>
@@ -2146,7 +2146,7 @@
         <v>39</v>
       </c>
       <c r="B93" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C93" t="s">
         <v>83</v>
@@ -2160,7 +2160,7 @@
         <v>40</v>
       </c>
       <c r="B94" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C94" t="s">
         <v>83</v>
@@ -2174,7 +2174,7 @@
         <v>41</v>
       </c>
       <c r="B95" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C95" t="s">
         <v>83</v>
@@ -2188,7 +2188,7 @@
         <v>42</v>
       </c>
       <c r="B96" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C96" t="s">
         <v>83</v>
@@ -2205,7 +2205,7 @@
         <v>43</v>
       </c>
       <c r="B97" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C97" t="s">
         <v>83</v>
@@ -2219,7 +2219,7 @@
         <v>44</v>
       </c>
       <c r="B98" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C98" t="s">
         <v>83</v>
@@ -2233,7 +2233,7 @@
         <v>45</v>
       </c>
       <c r="B99" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C99" t="s">
         <v>83</v>
@@ -2247,7 +2247,7 @@
         <v>46</v>
       </c>
       <c r="B100" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C100" t="s">
         <v>83</v>
@@ -2261,7 +2261,7 @@
         <v>47</v>
       </c>
       <c r="B101" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C101" t="s">
         <v>83</v>
@@ -2275,7 +2275,7 @@
         <v>48</v>
       </c>
       <c r="B102" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C102" t="s">
         <v>83</v>
@@ -2289,7 +2289,7 @@
         <v>49</v>
       </c>
       <c r="B103" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C103" t="s">
         <v>83</v>
@@ -2303,7 +2303,7 @@
         <v>50</v>
       </c>
       <c r="B104" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C104" t="s">
         <v>83</v>
@@ -2317,7 +2317,7 @@
         <v>51</v>
       </c>
       <c r="B105" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C105" t="s">
         <v>83</v>
@@ -2331,7 +2331,7 @@
         <v>52</v>
       </c>
       <c r="B106" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C106" t="s">
         <v>83</v>
@@ -2345,7 +2345,7 @@
         <v>53</v>
       </c>
       <c r="B107" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C107" t="s">
         <v>83</v>
@@ -2362,7 +2362,7 @@
         <v>54</v>
       </c>
       <c r="B108" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C108" t="s">
         <v>83</v>
@@ -2379,7 +2379,7 @@
         <v>55</v>
       </c>
       <c r="B109" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C109" t="s">
         <v>83</v>
@@ -2393,7 +2393,7 @@
         <v>56</v>
       </c>
       <c r="B110" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C110" t="s">
         <v>83</v>
@@ -2407,7 +2407,7 @@
         <v>57</v>
       </c>
       <c r="B111" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C111" t="s">
         <v>83</v>
@@ -2421,7 +2421,7 @@
         <v>58</v>
       </c>
       <c r="B112" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C112" t="s">
         <v>83</v>
@@ -2435,7 +2435,7 @@
         <v>59</v>
       </c>
       <c r="B113" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C113" t="s">
         <v>83</v>
@@ -2446,10 +2446,10 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B114" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C114" t="s">
         <v>83</v>
@@ -2463,7 +2463,7 @@
         <v>61</v>
       </c>
       <c r="B115" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C115" t="s">
         <v>83</v>
@@ -2477,7 +2477,7 @@
         <v>62</v>
       </c>
       <c r="B116" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C116" t="s">
         <v>83</v>
@@ -2491,7 +2491,7 @@
         <v>63</v>
       </c>
       <c r="B117" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C117" t="s">
         <v>83</v>
@@ -2505,7 +2505,7 @@
         <v>65</v>
       </c>
       <c r="B118" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C118" t="s">
         <v>83</v>
@@ -2516,10 +2516,10 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B119" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C119" t="s">
         <v>83</v>
@@ -2530,10 +2530,10 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B120" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C120" t="s">
         <v>83</v>
@@ -2544,10 +2544,10 @@
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B121" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C121" t="s">
         <v>83</v>
@@ -2558,10 +2558,10 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B122" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C122" t="s">
         <v>83</v>
@@ -2572,10 +2572,10 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B123" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C123" t="s">
         <v>83</v>
@@ -2586,10 +2586,10 @@
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B124" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C124" t="s">
         <v>83</v>
@@ -2600,10 +2600,10 @@
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B125" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C125" t="s">
         <v>83</v>
@@ -2614,10 +2614,10 @@
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B126" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C126" t="s">
         <v>83</v>
@@ -2628,10 +2628,10 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B127" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C127" t="s">
         <v>83</v>
@@ -2642,10 +2642,10 @@
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B128" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C128" t="s">
         <v>83</v>
@@ -2656,10 +2656,10 @@
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B129" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C129" t="s">
         <v>83</v>
@@ -2670,10 +2670,10 @@
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B130" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C130" t="s">
         <v>83</v>
@@ -2684,10 +2684,10 @@
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B131" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C131" t="s">
         <v>83</v>
@@ -2698,10 +2698,10 @@
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B132" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C132" t="s">
         <v>83</v>

</xml_diff>